<commit_message>
Default video PWM is 80 instead of 100; changes in NC_Bluetooth sketches
</commit_message>
<xml_diff>
--- a/Measures/NC_Bluetooth400/pwm2speed.xlsx
+++ b/Measures/NC_Bluetooth400/pwm2speed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\RotatingTable.Arduino\Measures\NC_Bluetooth400\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EE19B0-0CD0-4C1C-A38D-B59ED3D7F0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB07187-48A9-411C-B517-F8B033D39805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{A8659596-E7CE-445D-A5F7-DEEAE94F9AC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A8659596-E7CE-445D-A5F7-DEEAE94F9AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="24000 Гц Exact" sheetId="3" r:id="rId1"/>
@@ -82,10 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -197,85 +198,85 @@
             <c:numRef>
               <c:f>'24000 Гц Exact'!$B$2:$B$27</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>46.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>36.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>29.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>24.58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>21.58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>18.98</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>17.16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>15.65</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>14.18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>13.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>12.23</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>11.51</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11</c:v>
+                  <c:v>10.77</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>10.29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>9.6300000000000008</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9</c:v>
+                  <c:v>8.74</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8</c:v>
+                  <c:v>8.36</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8</c:v>
+                  <c:v>7.74</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>7.38</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7</c:v>
+                  <c:v>7.11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7</c:v>
+                  <c:v>6.87</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7</c:v>
+                  <c:v>6.64</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6</c:v>
+                  <c:v>6.39</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6</c:v>
+                  <c:v>6.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -495,7 +496,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1481,7 +1482,7 @@
   <dimension ref="A1:B197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B27"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,151 +1502,151 @@
       <c r="A2">
         <v>65</v>
       </c>
-      <c r="B2" s="2">
-        <v>48</v>
+      <c r="B2" s="3">
+        <v>46.6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>66</v>
       </c>
-      <c r="B3" s="2">
-        <v>37</v>
+      <c r="B3" s="3">
+        <v>36.04</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>67</v>
       </c>
-      <c r="B4" s="2">
-        <v>30</v>
+      <c r="B4" s="3">
+        <v>29.35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>68</v>
       </c>
-      <c r="B5" s="2">
-        <v>25</v>
+      <c r="B5" s="3">
+        <v>24.58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>69</v>
       </c>
-      <c r="B6" s="2">
-        <v>22</v>
+      <c r="B6" s="3">
+        <v>21.58</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>70</v>
       </c>
-      <c r="B7" s="2">
-        <v>19</v>
+      <c r="B7" s="3">
+        <v>18.98</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>71</v>
       </c>
-      <c r="B8" s="2">
-        <v>17</v>
+      <c r="B8" s="3">
+        <v>17.16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>72</v>
       </c>
-      <c r="B9" s="2">
-        <v>16</v>
+      <c r="B9" s="3">
+        <v>15.65</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>73</v>
       </c>
-      <c r="B10" s="2">
-        <v>14</v>
+      <c r="B10" s="3">
+        <v>14.18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>74</v>
       </c>
-      <c r="B11" s="2">
-        <v>13</v>
+      <c r="B11" s="3">
+        <v>13.2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>75</v>
       </c>
-      <c r="B12" s="2">
-        <v>12</v>
+      <c r="B12" s="3">
+        <v>12.23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>76</v>
       </c>
-      <c r="B13" s="2">
-        <v>12</v>
+      <c r="B13" s="3">
+        <v>11.51</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>77</v>
       </c>
-      <c r="B14" s="2">
-        <v>11</v>
+      <c r="B14" s="3">
+        <v>10.77</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>78</v>
       </c>
-      <c r="B15" s="2">
-        <v>10</v>
+      <c r="B15" s="3">
+        <v>10.29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>79</v>
       </c>
-      <c r="B16" s="2">
-        <v>10</v>
+      <c r="B16" s="3">
+        <v>9.6300000000000008</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>80</v>
       </c>
-      <c r="B17" s="2">
-        <v>9</v>
+      <c r="B17" s="3">
+        <v>9.18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>81</v>
       </c>
-      <c r="B18" s="2">
-        <v>9</v>
+      <c r="B18" s="3">
+        <v>8.74</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>82</v>
       </c>
-      <c r="B19" s="2">
-        <v>8</v>
+      <c r="B19" s="3">
+        <v>8.36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>83</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>8</v>
       </c>
     </row>
@@ -1653,119 +1654,169 @@
       <c r="A21">
         <v>84</v>
       </c>
-      <c r="B21" s="2">
-        <v>8</v>
+      <c r="B21" s="3">
+        <v>7.74</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>85</v>
       </c>
-      <c r="B22" s="2">
-        <v>7</v>
+      <c r="B22" s="3">
+        <v>7.38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>86</v>
       </c>
-      <c r="B23" s="2">
-        <v>7</v>
+      <c r="B23" s="3">
+        <v>7.11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>87</v>
       </c>
-      <c r="B24" s="2">
-        <v>7</v>
+      <c r="B24" s="3">
+        <v>6.87</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>88</v>
       </c>
-      <c r="B25" s="2">
-        <v>7</v>
+      <c r="B25" s="3">
+        <v>6.64</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>89</v>
       </c>
-      <c r="B26" s="2">
-        <v>6</v>
+      <c r="B26" s="3">
+        <v>6.39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>90</v>
       </c>
-      <c r="B27" s="2">
-        <v>6</v>
+      <c r="B27" s="3">
+        <v>6.22</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
+      <c r="A28">
+        <v>91</v>
+      </c>
+      <c r="B28" s="3">
+        <v>6.04</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
+      <c r="A29">
+        <v>92</v>
+      </c>
+      <c r="B29" s="3">
+        <v>5.93</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
+      <c r="A30">
+        <v>93</v>
+      </c>
+      <c r="B30" s="3">
+        <v>5.73</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="A31">
+        <v>94</v>
+      </c>
+      <c r="B31" s="3">
+        <v>5.53</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>95</v>
+      </c>
+      <c r="B32" s="3">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>96</v>
+      </c>
+      <c r="B33" s="3">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>97</v>
+      </c>
+      <c r="B34" s="3">
+        <v>5.14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>98</v>
+      </c>
+      <c r="B35" s="3">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>99</v>
+      </c>
+      <c r="B36" s="3">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>100</v>
+      </c>
+      <c r="B37" s="3">
+        <v>4.78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>